<commit_message>
year of cost calculation added
</commit_message>
<xml_diff>
--- a/Costs_Export_20250921_0158.xlsx
+++ b/Costs_Export_20250921_0158.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://burohappold-my.sharepoint.com/personal/arthur_emig_burohappold_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\000_cost_app\CostCatalogueBH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_B8A5257E8060956918156D88E9C160B081EECDDF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38A54558-B574-4764-986D-1F1F48070A2A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FF3CCB-3C42-4BA8-8497-BBBD3CF5416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="24600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="190">
   <si>
     <t>Include</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>Outdoor Technical Installations</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -1095,25 +1098,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="A53:XFD53"/>
+      <selection pane="bottomLeft" activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="18" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1168,8 +1171,11 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1224,8 +1230,11 @@
       <c r="R2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -1280,8 +1289,11 @@
       <c r="R3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -1336,8 +1348,11 @@
       <c r="R4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -1392,8 +1407,11 @@
       <c r="R5">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1448,8 +1466,11 @@
       <c r="R6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T6">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -1504,8 +1525,11 @@
       <c r="R7">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -1560,8 +1584,11 @@
       <c r="R8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T8">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -1616,8 +1643,11 @@
       <c r="R9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -1672,8 +1702,11 @@
       <c r="R10">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -1728,8 +1761,11 @@
       <c r="R11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T11">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -1784,8 +1820,11 @@
       <c r="R12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -1840,8 +1879,11 @@
       <c r="R13">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T13">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -1896,8 +1938,11 @@
       <c r="R14">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>1</v>
       </c>
@@ -1952,8 +1997,11 @@
       <c r="R15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>1</v>
       </c>
@@ -2008,8 +2056,11 @@
       <c r="R16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -2064,8 +2115,11 @@
       <c r="R17">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T17">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -2120,8 +2174,11 @@
       <c r="R18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T18">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -2176,8 +2233,11 @@
       <c r="R19">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T19">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -2232,8 +2292,11 @@
       <c r="R20">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T20">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>1</v>
       </c>
@@ -2288,8 +2351,11 @@
       <c r="R21">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T21">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -2344,8 +2410,11 @@
       <c r="R22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T22">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -2400,8 +2469,11 @@
       <c r="R23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -2456,8 +2528,11 @@
       <c r="R24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>1</v>
       </c>
@@ -2512,8 +2587,11 @@
       <c r="R25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T25">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -2568,8 +2646,11 @@
       <c r="R26">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T26">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -2624,8 +2705,11 @@
       <c r="R27">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T27">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -2680,8 +2764,11 @@
       <c r="R28">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T28">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="b">
         <v>1</v>
       </c>
@@ -2736,8 +2823,11 @@
       <c r="R29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T29">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -2792,8 +2882,11 @@
       <c r="R30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T30">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -2848,8 +2941,11 @@
       <c r="R31">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T31">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="b">
         <v>1</v>
       </c>
@@ -2904,8 +3000,11 @@
       <c r="R32">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T32">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="b">
         <v>1</v>
       </c>
@@ -2960,8 +3059,11 @@
       <c r="R33">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T33">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="b">
         <v>1</v>
       </c>
@@ -3016,8 +3118,11 @@
       <c r="R34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T34">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="b">
         <v>1</v>
       </c>
@@ -3072,8 +3177,11 @@
       <c r="R35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T35">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="b">
         <v>1</v>
       </c>
@@ -3128,8 +3236,11 @@
       <c r="R36">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T36">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="b">
         <v>1</v>
       </c>
@@ -3184,8 +3295,11 @@
       <c r="R37">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T37">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="b">
         <v>1</v>
       </c>
@@ -3240,8 +3354,11 @@
       <c r="R38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T38">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="b">
         <v>1</v>
       </c>
@@ -3296,8 +3413,11 @@
       <c r="R39">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T39">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="b">
         <v>1</v>
       </c>
@@ -3352,8 +3472,11 @@
       <c r="R40">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="b">
         <v>1</v>
       </c>
@@ -3408,8 +3531,11 @@
       <c r="R41">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T41">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="b">
         <v>1</v>
       </c>
@@ -3464,8 +3590,11 @@
       <c r="R42">
         <v>24</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T42">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="b">
         <v>1</v>
       </c>
@@ -3520,8 +3649,11 @@
       <c r="R43">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T43">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="b">
         <v>1</v>
       </c>
@@ -3576,8 +3708,11 @@
       <c r="R44">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T44">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="b">
         <v>1</v>
       </c>
@@ -3632,8 +3767,11 @@
       <c r="R45">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T45">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="b">
         <v>1</v>
       </c>
@@ -3688,8 +3826,11 @@
       <c r="R46">
         <v>18</v>
       </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T46">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="b">
         <v>1</v>
       </c>
@@ -3744,8 +3885,11 @@
       <c r="R47">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T47">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="b">
         <v>1</v>
       </c>
@@ -3800,8 +3944,11 @@
       <c r="R48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T48">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="b">
         <v>1</v>
       </c>
@@ -3856,8 +4003,11 @@
       <c r="R49">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T49">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="b">
         <v>1</v>
       </c>
@@ -3912,8 +4062,11 @@
       <c r="R50">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T50">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="b">
         <v>1</v>
       </c>
@@ -3967,6 +4120,9 @@
       </c>
       <c r="R51">
         <v>23</v>
+      </c>
+      <c r="T51">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -3980,17 +4136,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
@@ -4010,7 +4166,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>163</v>
       </c>
@@ -4030,7 +4186,7 @@
         <v>82.17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>165</v>
       </c>
@@ -4050,7 +4206,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>167</v>
       </c>
@@ -4070,7 +4226,7 @@
         <v>20.77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>169</v>
       </c>
@@ -4090,7 +4246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>171</v>
       </c>
@@ -4110,7 +4266,7 @@
         <v>20.46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>173</v>
       </c>
@@ -4130,7 +4286,7 @@
         <v>9.15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>175</v>
       </c>
@@ -4150,7 +4306,7 @@
         <v>18.09</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>177</v>
       </c>
@@ -4170,7 +4326,7 @@
         <v>17.79</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>179</v>
       </c>
@@ -4190,7 +4346,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>181</v>
       </c>
@@ -4210,7 +4366,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>183</v>
       </c>
@@ -4230,7 +4386,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>185</v>
       </c>
@@ -4250,7 +4406,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>187</v>
       </c>

</xml_diff>